<commit_message>
add Try Catch block
</commit_message>
<xml_diff>
--- a/Customers.xlsx
+++ b/Customers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\UiPath\ExcelCustomersToWebsite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060A5FB7-53D8-4A29-A5EA-50815B112B7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18743ED-1451-4A51-8085-A239A31E8CAE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14100" xr2:uid="{81F6032C-1B6A-4C79-B42C-4EA2C2677058}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -70,6 +70,26 @@
   </si>
   <si>
     <t>Sam@jones.com</t>
+  </si>
+  <si>
+    <t>Jack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reacher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Christian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -449,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795E5987-B860-4D91-AB00-D518042DEF23}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -462,7 +482,7 @@
     <col min="4" max="4" width="21.375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,10 +495,8 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -491,10 +509,8 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -507,10 +523,8 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -523,8 +537,31 @@
       <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -532,8 +569,9 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{CD9DDCC2-E7F7-4024-AB08-15F996957394}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>